<commit_message>
Adăugare senzor temperatură + conectori; Crearea unor footprint-uri pentru componente
</commit_message>
<xml_diff>
--- a/Info/Componente.xlsx
+++ b/Info/Componente.xlsx
@@ -56,12 +56,6 @@
     <t>Preț total [RON]</t>
   </si>
   <si>
-    <t>EC11J12-15P30C-SW</t>
-  </si>
-  <si>
-    <t>Codor: incremental; SMD; 15imp/rotaţie; două semnale A şi B; 5mA</t>
-  </si>
-  <si>
     <t>BC847C.215</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>EC11E12-15P30C-SW</t>
+  </si>
+  <si>
+    <t>Codor: incremental; THT; 15imp/rotaţie; două semnale A şi B; 5mA</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -502,6 +502,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,12 +791,12 @@
   <dimension ref="B1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -876,22 +879,22 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>10</v>
+      <c r="B7" s="31" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D7" s="11" t="str">
-        <f>HYPERLINK("https://www.tme.eu/ro/details/ec11j12-15p30c-sw/encodere-incrementale/sr-passives/ec11e12-15p30c-sw/","TME")</f>
+        <f>HYPERLINK("https://www.tme.eu/ro/details/ec11e12-15p30c-sw/encodere-incrementale/sr-passives/","TME")</f>
         <v>TME</v>
       </c>
       <c r="E7" s="11" t="str">
-        <f>HYPERLINK("https://www.tme.eu/Document/dab6de2c4798f6a842e4ac29271f1b9f/EC11J12-15P30C-SW.pdf","Link")</f>
+        <f>HYPERLINK("https://www.tme.eu/Document/44e8c47524c4eb6c460cbc7fca5d0c53/EC11E12-15P30C-SW.pdf","Link")</f>
         <v>Link</v>
       </c>
       <c r="F7" s="10">
-        <v>8.02</v>
+        <v>6.26</v>
       </c>
       <c r="G7" s="12">
         <v>1</v>
@@ -899,10 +902,10 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="11" t="str">
         <f>HYPERLINK("https://www.tme.eu/ro/details/bc847c.215/tranzistori-smd-npn/nexperia/","TME")</f>
@@ -919,10 +922,10 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="11" t="str">
         <f>HYPERLINK("https://www.tme.eu/ro/details/bc857c.215/tranzistori-smd-pnp/nexperia/","TME")</f>
@@ -939,20 +942,20 @@
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>18</v>
       </c>
       <c r="E10" s="17" t="str">
         <f>HYPERLINK("https://www.infineon.com/dgdl/Infineon-TLE4946_2L-DS-v01_00-en.pdf?fileId=db3a304338ec6d390138fc8f905876d3","Link")</f>
         <v>Link</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G10" s="18">
         <v>1</v>

</xml_diff>